<commit_message>
commit source test processTrigger
</commit_message>
<xml_diff>
--- a/List_Case/removeTrigger/removeTrigger_diagram.xlsx
+++ b/List_Case/removeTrigger/removeTrigger_diagram.xlsx
@@ -607,65 +607,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48:E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -978,747 +978,747 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17">
-      <c r="B2" s="4"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="15"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B5" s="5"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="18"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B6" s="5"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="18"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="5"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="2:17">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="2:17">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="2:17">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="2:17">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="2:17">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="2:17">
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="2:17">
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="2:17">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="2:17">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="23"/>
+      <c r="C21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="2:17">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
     </row>
     <row r="23" spans="2:17">
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="2:17">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
     </row>
     <row r="25" spans="2:17">
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="2:17">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
     </row>
     <row r="27" spans="2:17">
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
     </row>
     <row r="28" spans="2:17">
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
     </row>
     <row r="29" spans="2:17">
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
     </row>
     <row r="30" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
     </row>
     <row r="31" spans="2:17">
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
     </row>
     <row r="32" spans="2:17">
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
     </row>
     <row r="33" spans="2:17">
-      <c r="B33" s="5"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
     </row>
     <row r="34" spans="2:17">
-      <c r="B34" s="5"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="23"/>
+      <c r="C34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
     </row>
     <row r="35" spans="2:17">
-      <c r="B35" s="5"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
     </row>
     <row r="36" spans="2:17">
-      <c r="B36" s="5"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
     </row>
     <row r="37" spans="2:17">
-      <c r="B37" s="5"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
     </row>
     <row r="38" spans="2:17">
-      <c r="B38" s="5"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
     </row>
     <row r="39" spans="2:17">
-      <c r="B39" s="5"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1731,145 +1731,145 @@
       <c r="F39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="2:17">
-      <c r="B40" s="5"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="2:17">
-      <c r="B41" s="5"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="23"/>
-      <c r="N41" s="23"/>
-      <c r="O41" s="23"/>
-      <c r="P41" s="23"/>
-      <c r="Q41" s="23"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="2:17">
-      <c r="B42" s="5"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="2:17">
-      <c r="B43" s="5"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="2:17">
-      <c r="B44" s="5"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
     </row>
     <row r="45" spans="2:17">
-      <c r="B45" s="5"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="23"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="23"/>
-      <c r="Q45" s="23"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="2:17">
-      <c r="B46" s="5"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
     </row>
     <row r="48" spans="2:17">
       <c r="E48" s="2" t="s">
@@ -1885,17 +1885,22 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="E39:E46"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="D39:D46"/>
-    <mergeCell ref="G30:Q33"/>
-    <mergeCell ref="G34:Q38"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="F34:F38"/>
-    <mergeCell ref="F39:F46"/>
-    <mergeCell ref="G39:Q46"/>
+    <mergeCell ref="C39:C46"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B29"/>
+    <mergeCell ref="D34:D38"/>
+    <mergeCell ref="B30:B46"/>
+    <mergeCell ref="C21:C29"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="E12:E20"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C20"/>
+    <mergeCell ref="D4:D7"/>
     <mergeCell ref="G2:Q3"/>
     <mergeCell ref="G12:Q20"/>
     <mergeCell ref="D21:D29"/>
@@ -1912,22 +1917,17 @@
     <mergeCell ref="F12:F20"/>
     <mergeCell ref="F21:F29"/>
     <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E12:E20"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C20"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="C39:C46"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B29"/>
-    <mergeCell ref="D34:D38"/>
-    <mergeCell ref="B30:B46"/>
-    <mergeCell ref="C21:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="G30:Q33"/>
+    <mergeCell ref="G34:Q38"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="F39:F46"/>
+    <mergeCell ref="G39:Q46"/>
+    <mergeCell ref="E39:E46"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="D39:D46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>